<commit_message>
Change workload xls file
Signed-off-by: Atul Deshmukh <atul.deshmukh@seagate.com>
</commit_message>
<xml_diff>
--- a/scripts/workload/sample_workload_excel.xlsx
+++ b/scripts/workload/sample_workload_excel.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC28C7B6-C278-40B2-B42A-C7088D03FC87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Seagate_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC387E3-039B-4388-A317-290AD2CA4C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workloads" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <sheet name="MOTR_CONFIG" sheetId="2" r:id="rId7"/>
     <sheet name="singlenode_param" sheetId="4" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="125">
   <si>
     <t>CMND</t>
   </si>
@@ -404,13 +409,16 @@
   </si>
   <si>
     <t>/etc/motr/conf.xc</t>
+  </si>
+  <si>
+    <t>sleep</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -776,28 +784,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="5"/>
-    <col min="5" max="5" width="7.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="5"/>
-    <col min="10" max="10" width="12.7109375" style="5" customWidth="1"/>
-    <col min="11" max="27" width="9.140625" style="5"/>
+    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="5"/>
+    <col min="5" max="5" width="7.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="5"/>
+    <col min="10" max="10" width="12.6640625" style="5" customWidth="1"/>
+    <col min="11" max="27" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="33.75">
+    <row r="1" spans="1:27" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -880,7 +888,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="56.25">
+    <row r="2" spans="1:27" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -898,7 +906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="22.5">
+    <row r="3" spans="1:27" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -922,29 +930,25 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="2">
-        <v>512</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="2">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="22.5">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -958,207 +962,450 @@
       <c r="F5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="K6" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2">
+        <v>512</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P7" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="45">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="K8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:27" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:27" ht="33.75">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:27" ht="45">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:27">
-      <c r="A9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="K10" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P11" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="P12" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="K12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:27">
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="K14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="K16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P17" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="K18" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P19" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="K20" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="K22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="K24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="67.5">
-      <c r="A16" s="1" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="K26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B27" s="1">
         <v>3</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K27" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="K28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B29" s="1">
         <v>3</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="1">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="K30" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B31" s="1">
         <v>4</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="K32" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B33" s="1">
         <v>5</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K008000Seagate Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1166,27 +1413,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86561E2-F3CC-4E57-A403-947397189A11}">
   <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="19.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="6" max="7" width="9.140625" style="3"/>
-    <col min="8" max="14" width="9.140625" style="4"/>
-    <col min="15" max="16" width="9.140625" style="3"/>
-    <col min="17" max="18" width="9.140625" style="4"/>
-    <col min="19" max="19" width="9.140625" style="5"/>
-    <col min="20" max="28" width="9.140625" style="2"/>
-    <col min="29" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="19.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="3"/>
+    <col min="5" max="5" width="9.109375" style="4"/>
+    <col min="6" max="7" width="9.109375" style="3"/>
+    <col min="8" max="14" width="9.109375" style="4"/>
+    <col min="15" max="16" width="9.109375" style="3"/>
+    <col min="17" max="18" width="9.109375" style="4"/>
+    <col min="19" max="19" width="9.109375" style="5"/>
+    <col min="20" max="28" width="9.109375" style="2"/>
+    <col min="29" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="22.5">
+    <row r="1" spans="1:33" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1287,7 +1534,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1348,7 +1595,7 @@
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1412,7 +1659,7 @@
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1473,7 +1720,7 @@
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1537,7 +1784,7 @@
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1601,7 +1848,7 @@
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>2</v>
       </c>
@@ -1665,7 +1912,7 @@
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -1729,7 +1976,7 @@
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>4</v>
       </c>
@@ -1793,7 +2040,7 @@
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>5</v>
       </c>
@@ -1857,6 +2104,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K008000Seagate Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1865,15 +2116,15 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="1" max="2" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1881,23 +2132,23 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>108</v>
       </c>
@@ -1905,7 +2156,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>98</v>
       </c>
@@ -1913,7 +2164,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>87</v>
       </c>
@@ -1923,6 +2174,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K008000Seagate Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1932,23 +2187,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="22.5">
+    <row r="2" spans="1:1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K008000Seagate Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1958,23 +2217,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K008000Seagate Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1986,12 +2249,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="1" max="2" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -2002,7 +2265,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="22.5">
+    <row r="2" spans="1:3" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>115</v>
       </c>
@@ -2013,12 +2276,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K008000Seagate Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2030,16 +2297,16 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="5" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="5"/>
-    <col min="7" max="7" width="11.7109375" style="5" customWidth="1"/>
-    <col min="8" max="11" width="9.140625" style="5"/>
+    <col min="1" max="1" width="13.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="5" customWidth="1"/>
+    <col min="3" max="6" width="9.109375" style="5"/>
+    <col min="7" max="7" width="11.6640625" style="5" customWidth="1"/>
+    <col min="8" max="11" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75">
+    <row r="1" spans="1:11" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -2074,7 +2341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="33.75">
+    <row r="2" spans="1:11" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -2111,6 +2378,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K008000Seagate Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2118,16 +2389,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507BE496-48A9-4B03-A554-40C56B8DC215}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="1" max="2" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>121</v>
       </c>
@@ -2135,7 +2406,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="22.5">
+    <row r="2" spans="1:2" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>123</v>
       </c>
@@ -2145,5 +2416,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K008000Seagate Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>